<commit_message>
kyon's Furniture Mediterranean - 3293528946 업데이트
</commit_message>
<xml_diff>
--- a/Data/kyon's Furniture Mediterranean - 3293528946/3293528946.xlsx
+++ b/Data/kyon's Furniture Mediterranean - 3293528946/3293528946.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Pull Request Here\kyon's Furniture地中海风格家具Mediterranean - 3293528946\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\kyon's Furniture Mediterranean - 3293528946\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB23707A-94E2-4719-BDF9-CD184577CFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B42FC7-DEBA-4FD3-ADCF-989BFAAB1797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_240925" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>bjmi0</author>
+  </authors>
+  <commentList>
+    <comment ref="E79" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-12-21에 새로 추가된 노드들 (8개)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F79" authorId="0" shapeId="0" xr:uid="{340F4277-706C-4E8F-B681-365B527BE727}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-12-21에 새로 추가된 노드들 (8개)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="327">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -365,471 +401,483 @@
     <t>Mediterranean_MetalFence.label</t>
   </si>
   <si>
+    <t>围栏a</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Cushion_a.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>지중해 울타리 A</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mediterranean_Cushion_a.label</t>
+  </si>
+  <si>
+    <t>抱枕a</t>
+  </si>
+  <si>
+    <t>지중해 흰색 베개</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Cushion_b.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Cushion_b.label</t>
+  </si>
+  <si>
+    <t>抱枕b</t>
+  </si>
+  <si>
+    <t>지중해 파란 베개</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_DessertBox.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_DessertBox.label</t>
+  </si>
+  <si>
+    <t>甜点盒</t>
+  </si>
+  <si>
+    <t>지중해 간식 상자</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Door_a.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Door_a.label</t>
+  </si>
+  <si>
+    <t>拱门a</t>
+  </si>
+  <si>
+    <t>지중해 문</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Door_b.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Door_b.label</t>
+  </si>
+  <si>
+    <t>拱门b</t>
+  </si>
+  <si>
+    <t>지중해 반투명 문</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_chair_A.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_chair_A.label</t>
+  </si>
+  <si>
+    <t>餐椅a</t>
+  </si>
+  <si>
+    <t>지중해 의자</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_chair_B.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_chair_B.label</t>
+  </si>
+  <si>
+    <t>餐椅b</t>
+  </si>
+  <si>
+    <t>지중해 의자 (대각선)</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Stool.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Stool.label</t>
+  </si>
+  <si>
+    <t>凳子</t>
+  </si>
+  <si>
+    <t>지중해 작은 의자</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_chair_C.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_chair_C.label</t>
+  </si>
+  <si>
+    <t>公园长椅</t>
+  </si>
+  <si>
+    <t>지중해 공원 의자</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_sofa_A.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_sofa_A.label</t>
+  </si>
+  <si>
+    <t>沙发a</t>
+  </si>
+  <si>
+    <t>지중해 큰 소파</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_sofa_B.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_sofa_B.label</t>
+  </si>
+  <si>
+    <t>沙发b</t>
+  </si>
+  <si>
+    <t>지중해 소파</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_DoubleBed.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_DoubleBed.label</t>
+  </si>
+  <si>
+    <t>双人床</t>
+  </si>
+  <si>
+    <t>지중해 큰 침대</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_SingleBed.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_SingleBed.label</t>
+  </si>
+  <si>
+    <t>单人床</t>
+  </si>
+  <si>
+    <t>지중해 침대</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_EndTable.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_EndTable.label</t>
+  </si>
+  <si>
+    <t>床头柜</t>
+  </si>
+  <si>
+    <t>지중해 수납장</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Wardrobe.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Wardrobe.label</t>
+  </si>
+  <si>
+    <t>衣柜</t>
+  </si>
+  <si>
+    <t>지중해 옷장</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Table_a.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Table_a.label</t>
+  </si>
+  <si>
+    <t>桌子1x2</t>
+  </si>
+  <si>
+    <t>지중해 책상 (1x2)</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Table_b.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Table_b.label</t>
+  </si>
+  <si>
+    <t>桌子1x3</t>
+  </si>
+  <si>
+    <t>지중해 책상 (1x3)</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Table_c.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Table_c.label</t>
+  </si>
+  <si>
+    <t>桌子2x3</t>
+  </si>
+  <si>
+    <t>지중해 책상 (2x3)</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Table_d.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Table_d.label</t>
+  </si>
+  <si>
+    <t>桌子1x1</t>
+  </si>
+  <si>
+    <t>지중해 책상 (1x1)</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Table_e.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Table_e.label</t>
+  </si>
+  <si>
+    <t>桌子1x1(桌布)</t>
+  </si>
+  <si>
+    <t>지중해 식탁보 책상 (1x1)</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Lounge.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Lounge.label</t>
+  </si>
+  <si>
+    <t>沙滩躺椅</t>
+  </si>
+  <si>
+    <t>지중해 해변 의자</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Lounge.description</t>
+  </si>
+  <si>
+    <t>Mediterranean_Lounge.description</t>
+  </si>
+  <si>
+    <t>懒狗，敬请见证</t>
+  </si>
+  <si>
+    <t>해변에서 으레 볼 수 있는 의자입니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Drape_a.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Drape_a.label</t>
+  </si>
+  <si>
+    <t>帘幕a</t>
+  </si>
+  <si>
+    <t>지중해 커튼 (닫힘)</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Drape_b.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Drape_b.label</t>
+  </si>
+  <si>
+    <t>帘幕b</t>
+  </si>
+  <si>
+    <t>지중해 커튼 (열림)</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_TableLamp.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_TableLamp.label</t>
+  </si>
+  <si>
+    <t>台灯</t>
+  </si>
+  <si>
+    <t>지중해 책상등</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_WallLight.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_WallLight.label</t>
+  </si>
+  <si>
+    <t>壁灯</t>
+  </si>
+  <si>
+    <t>지중해 벽등</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_StreetLight.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_StreetLight.label</t>
+  </si>
+  <si>
+    <t>路灯</t>
+  </si>
+  <si>
+    <t>지중해 가로등</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_DoricOrder_a.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_DoricOrder_a.label</t>
+  </si>
+  <si>
+    <t>罗马柱a</t>
+  </si>
+  <si>
+    <t>지중해 양방향 기둥</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_DoricOrder_b.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_DoricOrder_b.label</t>
+  </si>
+  <si>
+    <t>罗马柱b</t>
+  </si>
+  <si>
+    <t>지중해 단방향 기둥</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_PlantPot_a.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_PlantPot_a.label</t>
+  </si>
+  <si>
+    <t>植物隔板</t>
+  </si>
+  <si>
+    <t>지중해 화분</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Wall_a.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Wall_a.label</t>
+  </si>
+  <si>
+    <t>地中海白墙</t>
+  </si>
+  <si>
+    <t>지중해 흰색 벽</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Wall_a.description</t>
+  </si>
+  <si>
+    <t>Mediterranean_Wall_a.description</t>
+  </si>
+  <si>
+    <t>一面无法通过的墙。可以支撑起屋顶。</t>
+  </si>
+  <si>
+    <t>지나갈 수 없는 벽입니다. 지붕을 지지할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Wall_b.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Wall_b.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Wall_b.description</t>
+  </si>
+  <si>
+    <t>Mediterranean_Wall_b.description</t>
+  </si>
+  <si>
+    <t>无透视差分</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Wall_c.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Wall_c.label</t>
+  </si>
+  <si>
+    <t>地中海砖墙</t>
+  </si>
+  <si>
+    <t>지중해 벽돌 벽</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Wall_c.description</t>
+  </si>
+  <si>
+    <t>Mediterranean_Wall_c.description</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Wall_d.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Wall_d.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Wall_d.description</t>
+  </si>
+  <si>
+    <t>Mediterranean_Wall_d.description</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Wall_e.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Wall_e.label</t>
+  </si>
+  <si>
+    <t>皮兰色墙</t>
+  </si>
+  <si>
+    <t>지중해 피라미드 벽</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Wall_e.description</t>
+  </si>
+  <si>
+    <t>Mediterranean_Wall_e.description</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Wall_f.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Wall_f.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Wall_f.description</t>
+  </si>
+  <si>
+    <t>Mediterranean_Wall_f.description</t>
+  </si>
+  <si>
     <t>ThingDef+Mediterranean_WoodFence.label</t>
   </si>
   <si>
-    <t>ThingDef+Mediterranean_Cushion_a.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Cushion_a.label</t>
-  </si>
-  <si>
-    <t>抱枕a</t>
-  </si>
-  <si>
-    <t>지중해 흰색 베개</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Cushion_b.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Cushion_b.label</t>
-  </si>
-  <si>
-    <t>抱枕b</t>
-  </si>
-  <si>
-    <t>지중해 파란 베개</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_DessertBox.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_DessertBox.label</t>
-  </si>
-  <si>
-    <t>甜点盒</t>
-  </si>
-  <si>
-    <t>지중해 간식 상자</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Door_a.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Door_a.label</t>
-  </si>
-  <si>
-    <t>拱门a</t>
-  </si>
-  <si>
-    <t>지중해 문</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Door_b.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Door_b.label</t>
-  </si>
-  <si>
-    <t>拱门b</t>
-  </si>
-  <si>
-    <t>지중해 반투명 문</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_chair_A.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_chair_A.label</t>
-  </si>
-  <si>
-    <t>餐椅a</t>
-  </si>
-  <si>
-    <t>지중해 의자</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_chair_B.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_chair_B.label</t>
-  </si>
-  <si>
-    <t>餐椅b</t>
-  </si>
-  <si>
-    <t>지중해 의자 (대각선)</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Stool.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Stool.label</t>
-  </si>
-  <si>
-    <t>凳子</t>
-  </si>
-  <si>
-    <t>지중해 작은 의자</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_chair_C.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_chair_C.label</t>
-  </si>
-  <si>
-    <t>公园长椅</t>
-  </si>
-  <si>
-    <t>지중해 공원 의자</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_sofa_A.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_sofa_A.label</t>
-  </si>
-  <si>
-    <t>沙发a</t>
-  </si>
-  <si>
-    <t>지중해 큰 소파</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_sofa_B.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_sofa_B.label</t>
-  </si>
-  <si>
-    <t>沙发b</t>
-  </si>
-  <si>
-    <t>지중해 소파</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_DoubleBed.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_DoubleBed.label</t>
-  </si>
-  <si>
-    <t>双人床</t>
-  </si>
-  <si>
-    <t>지중해 큰 침대</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_SingleBed.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_SingleBed.label</t>
-  </si>
-  <si>
-    <t>单人床</t>
-  </si>
-  <si>
-    <t>지중해 침대</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_EndTable.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_EndTable.label</t>
-  </si>
-  <si>
-    <t>床头柜</t>
-  </si>
-  <si>
-    <t>지중해 수납장</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Wardrobe.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Wardrobe.label</t>
-  </si>
-  <si>
-    <t>衣柜</t>
-  </si>
-  <si>
-    <t>지중해 옷장</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Table_a.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Table_a.label</t>
-  </si>
-  <si>
-    <t>桌子1x2</t>
-  </si>
-  <si>
-    <t>지중해 책상 (1x2)</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Table_b.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Table_b.label</t>
-  </si>
-  <si>
-    <t>桌子1x3</t>
-  </si>
-  <si>
-    <t>지중해 책상 (1x3)</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Table_c.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Table_c.label</t>
-  </si>
-  <si>
-    <t>桌子2x3</t>
-  </si>
-  <si>
-    <t>지중해 책상 (2x3)</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Table_d.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Table_d.label</t>
-  </si>
-  <si>
-    <t>桌子1x1</t>
-  </si>
-  <si>
-    <t>지중해 책상 (1x1)</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Table_e.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Table_e.label</t>
-  </si>
-  <si>
-    <t>桌子1x1(桌布)</t>
-  </si>
-  <si>
-    <t>지중해 식탁보 책상 (1x1)</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Lounge.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Lounge.label</t>
-  </si>
-  <si>
-    <t>沙滩躺椅</t>
-  </si>
-  <si>
-    <t>지중해 해변 의자</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Lounge.description</t>
-  </si>
-  <si>
-    <t>Mediterranean_Lounge.description</t>
-  </si>
-  <si>
-    <t>懒狗，敬请见证</t>
-  </si>
-  <si>
-    <t>해변에서 으레 볼 수 있는 의자입니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Drape_a.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Drape_a.label</t>
-  </si>
-  <si>
-    <t>帘幕a</t>
-  </si>
-  <si>
-    <t>지중해 커튼 (닫힘)</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Drape_b.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Drape_b.label</t>
-  </si>
-  <si>
-    <t>帘幕b</t>
-  </si>
-  <si>
-    <t>지중해 커튼 (열림)</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_TableLamp.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_TableLamp.label</t>
-  </si>
-  <si>
-    <t>台灯</t>
-  </si>
-  <si>
-    <t>지중해 책상등</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_WallLight.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_WallLight.label</t>
-  </si>
-  <si>
-    <t>壁灯</t>
-  </si>
-  <si>
-    <t>지중해 벽등</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_StreetLight.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_StreetLight.label</t>
-  </si>
-  <si>
-    <t>路灯</t>
-  </si>
-  <si>
-    <t>지중해 가로등</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_DoricOrder_a.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_DoricOrder_a.label</t>
-  </si>
-  <si>
-    <t>罗马柱a</t>
-  </si>
-  <si>
-    <t>지중해 양방향 기둥</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_DoricOrder_b.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_DoricOrder_b.label</t>
-  </si>
-  <si>
-    <t>罗马柱b</t>
-  </si>
-  <si>
-    <t>지중해 단방향 기둥</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_PlantPot_a.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_PlantPot_a.label</t>
-  </si>
-  <si>
-    <t>植物隔板</t>
-  </si>
-  <si>
-    <t>지중해 화분</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Wall_a.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Wall_a.label</t>
-  </si>
-  <si>
-    <t>地中海白墙</t>
-  </si>
-  <si>
-    <t>지중해 흰색 벽</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Wall_a.description</t>
-  </si>
-  <si>
-    <t>Mediterranean_Wall_a.description</t>
-  </si>
-  <si>
-    <t>一面无法通过的墙。可以支撑起屋顶。</t>
-  </si>
-  <si>
-    <t>지나갈 수 없는 벽입니다. 지붕을 지지할 수 있습니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Wall_b.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Wall_b.label</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Wall_b.description</t>
-  </si>
-  <si>
-    <t>Mediterranean_Wall_b.description</t>
-  </si>
-  <si>
-    <t>无透视差分</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Wall_c.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Wall_c.label</t>
-  </si>
-  <si>
-    <t>地中海砖墙</t>
-  </si>
-  <si>
-    <t>지중해 벽돌 벽</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Wall_c.description</t>
-  </si>
-  <si>
-    <t>Mediterranean_Wall_c.description</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Wall_d.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Wall_d.label</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Wall_d.description</t>
-  </si>
-  <si>
-    <t>Mediterranean_Wall_d.description</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Wall_e.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Wall_e.label</t>
-  </si>
-  <si>
-    <t>皮兰色墙</t>
-  </si>
-  <si>
-    <t>지중해 피라미드 벽</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Wall_e.description</t>
-  </si>
-  <si>
-    <t>Mediterranean_Wall_e.description</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Wall_f.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Wall_f.label</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Wall_f.description</t>
-  </si>
-  <si>
-    <t>Mediterranean_Wall_f.description</t>
-  </si>
-  <si>
-    <t>围栏a</t>
-  </si>
-  <si>
     <t>Mediterranean_WoodFence.label</t>
   </si>
   <si>
@@ -839,36 +887,28 @@
     <t>ThingDef+Mediterranean_Dresser.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>지중해 울타리 B</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Mediterranean_Dresser.label</t>
   </si>
   <si>
-    <t>ThingDef+Mediterranean_Carton_a.label</t>
-  </si>
-  <si>
-    <t>Mediterranean_Carton_a.label</t>
-  </si>
-  <si>
-    <t>Adaptive Storage Framework</t>
-  </si>
-  <si>
-    <t>纸板箱a</t>
-  </si>
-  <si>
-    <t>ThingDef+Mediterranean_Carton_b.label</t>
-  </si>
-  <si>
-    <t>纸板箱b</t>
-  </si>
-  <si>
-    <t>지중해 울타리 B</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>지중해 울타리 A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
       <t>梳</t>
     </r>
     <r>
@@ -877,7 +917,6 @@
         <color rgb="FF000000"/>
         <rFont val="Microsoft JhengHei"/>
         <family val="2"/>
-        <charset val="136"/>
       </rPr>
       <t>妆</t>
     </r>
@@ -890,29 +929,226 @@
       </rPr>
       <t>台</t>
     </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>지중해 옷장</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Carton_a.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Carton_a.label</t>
+  </si>
+  <si>
+    <t>Adaptive Storage Framework</t>
+  </si>
+  <si>
+    <t>纸板箱a</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Carton_b.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>지중해 상자 A</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>纸板箱b</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>Mediterranean_Carton_b.label</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>金属围栏</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>지중해 상자 B</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>지중해 울타리</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Window_c.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Window_c.label</t>
+  </si>
+  <si>
+    <t>落地窗c</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Window_c.description</t>
+  </si>
+  <si>
+    <t>Mediterranean_Window_c.description</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Door_c.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Door_c.label</t>
+  </si>
+  <si>
+    <t>拱门c</t>
+  </si>
+  <si>
+    <t>ThingDef+Mediterranean_Door_c.description</t>
+  </si>
+  <si>
+    <t>Mediterranean_Door_c.description</t>
+  </si>
+  <si>
+    <t>自动门</t>
+  </si>
+  <si>
+    <t>TerrainDef+Mediterranean_Tile_a.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Tile_a.label</t>
+  </si>
+  <si>
+    <t>白色瓷砖</t>
+  </si>
+  <si>
+    <t>TerrainDef+Mediterranean_Tile_a.description</t>
+  </si>
+  <si>
+    <t>Mediterranean_Tile_a.description</t>
+  </si>
+  <si>
+    <t>----</t>
+  </si>
+  <si>
+    <t>TerrainDef+Mediterranean_Tile_b.label</t>
+  </si>
+  <si>
+    <t>Mediterranean_Tile_b.label</t>
+  </si>
+  <si>
+    <t>TerrainDef+Mediterranean_Tile_b.description</t>
+  </si>
+  <si>
+    <t>Mediterranean_Tile_b.description</t>
+  </si>
+  <si>
+    <t>지중해 대형 창문 C</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>지중해 옷장</t>
+    <t>경고: 바깥쪽으로 총을 쏘거나 통과하지 마세요.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Mediterranean_Carton_b.label</t>
+    <t>지중해 문 A</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>지중해 상자 A</t>
+    <t>지중해 문 B</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>지중해 상자 B</t>
+    <t>지중해 의자 A</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>지중해 울타리</t>
-  </si>
-  <si>
-    <t>金属围栏</t>
+    <t>지중해 의자 B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지중해 소파 A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지중해 소파 B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지중해 커튼 (닫힘)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지중해 기둥 A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지중해 기둥 B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지중해 문 C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지중해 자동문</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지중해의 하얀 바닥입니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>米色瓷</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="새굴림"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t>砖</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지중해 연갈색 바닥</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지중해 흰색 바닥</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>지중해 스타일의 베이지색 바닥입니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -943,20 +1179,18 @@
       <color rgb="FF000000"/>
       <name val="Microsoft JhengHei"/>
       <family val="2"/>
-      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
+      <name val="새굴림"/>
+      <family val="1"/>
       <charset val="129"/>
     </font>
   </fonts>
@@ -990,13 +1224,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1298,11 +1530,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F77"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1589,7 +1821,7 @@
         <v>66</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>67</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
@@ -1841,10 +2073,10 @@
         <v>113</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>268</v>
+        <v>114</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>280</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -1855,789 +2087,926 @@
         <v>26</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>130</v>
+        <v>311</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>134</v>
+        <v>312</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>138</v>
+        <v>313</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>142</v>
+        <v>314</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>154</v>
+        <v>315</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>158</v>
+        <v>316</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>206</v>
+        <v>317</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>226</v>
+        <v>318</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>230</v>
+        <v>319</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>114</v>
+        <v>269</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>279</v>
+        <v>271</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>284</v>
+        <v>280</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>278</v>
-      </c>
       <c r="F77" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A79" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A80" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A81" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A82" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A83" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A84" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A85" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A86" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>326</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2657,7 +3026,8 @@
     <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.7265625" style="1" customWidth="1"/>
     <col min="6" max="6" width="63.453125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="9.1796875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -3184,10 +3554,10 @@
         <v>113</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -3198,710 +3568,710 @@
         <v>26</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>